<commit_message>
feat: Implement Amazon ETL with T0007-T0022 tasks
- T0007: Basic CSV/Excel read/write operations
- T0008-T0017: Transform pipeline with cleaning utilities, data quality checks, aggregations, feature engineering
- T0018-T0022: Advanced load operations with bulk loading, incremental/full modes, constraint handling, upsert logic, and reject table
- Add comprehensive documentation in docs/Implementation_Snippets.md
- Add reusable utilities (cleaning_utils.py, config_loader.py)
- Add unit tests for utilities
- Update README with full project documentation
</commit_message>
<xml_diff>
--- a/data/processed/orders_summary.xlsx
+++ b/data/processed/orders_summary.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,29 +437,37 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>max_orders</t>
+          <t>total_orders</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>min_orders</t>
+          <t>max_quantity</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>total_orders</t>
+          <t>min_quantity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_quantity</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>149</v>
+        <v>79435</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>15593</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>238661</v>
       </c>
     </row>
   </sheetData>
@@ -473,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,55 +492,275 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>state</t>
+          <t>State</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>max_orders</t>
+          <t>total_orders</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>min_orders</t>
+          <t>max_quantity</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>total_orders</t>
+          <t>min_quantity</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>total_quantity</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Andhra Pradesh</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>149</v>
+        <v>3932</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>7805</v>
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>11849</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>149</v>
+        <v>15812</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>7788</v>
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>47298</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3991</v>
+      </c>
+      <c r="C4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12058</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DC</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>4001</v>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>11980</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FL</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4042</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12154</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4046</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>12150</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3968</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>11971</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NC</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4083</v>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>12415</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NY</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3886</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>11706</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>OH</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>3969</v>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="n">
+        <v>11965</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>PA</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>3980</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12036</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TX</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>19768</v>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="n">
+        <v>59198</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WA</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>3957</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="n">
+        <v>11881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>